<commit_message>
Actualizacion de info de locales
</commit_message>
<xml_diff>
--- a/Excel Locales/Horario apertura y cierre de Locales.xlsx
+++ b/Excel Locales/Horario apertura y cierre de Locales.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19980" windowHeight="7305"/>
+    <workbookView xWindow="240" yWindow="96" windowWidth="19980" windowHeight="7308"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -174,9 +174,6 @@
     <t>de 10 a 1330 y 1530 a 20 lu a sab</t>
   </si>
   <si>
-    <t>de 930 a 1300 y de 16 a 2030 lu a vie y sab de 10 a 14 y 1630 a 2030</t>
-  </si>
-  <si>
     <t>de 10 a 13 y de 16 a 20 lu a vie y sab de 10 a 14 y de 16 a 2030</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>de 10</t>
+  </si>
+  <si>
+    <t>de 930 a 1300 y de 16 a 2030 lu a vie y sab de 10 a 14 y 1630 a 20</t>
   </si>
 </sst>
 </file>
@@ -569,13 +569,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +853,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -892,7 +892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>